<commit_message>
Improved plate layout and removed extraneous data
</commit_message>
<xml_diff>
--- a/resources/templates/NOMADS_sWGA_Worksheet.xlsx
+++ b/resources/templates/NOMADS_sWGA_Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitrepos\warehouse\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C746D34-23B8-46A7-89EF-BCC414A2E9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B078DED3-B04B-4F2E-8A65-7E17EE911051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{202E2ACC-7D07-5944-B6D6-A1D8A2363375}"/>
   </bookViews>
@@ -1424,6 +1424,78 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1450,78 +1522,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2263,7 +2263,7 @@
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2272,176 +2272,176 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="68" t="s">
         <v>150</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="54" t="s">
         <v>137</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="64" t="s">
+      <c r="B2" s="55"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="69" t="s">
         <v>141</v>
       </c>
-      <c r="H2" s="64"/>
-      <c r="K2" s="56" t="s">
+      <c r="H2" s="69"/>
+      <c r="K2" s="80" t="s">
         <v>140</v>
       </c>
-      <c r="L2" s="56"/>
+      <c r="L2" s="80"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="54" t="s">
         <v>142</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
       <c r="G3" t="s">
         <v>147</v>
       </c>
-      <c r="K3" s="54" t="s">
+      <c r="K3" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="54"/>
+      <c r="L3" s="78"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="54" t="s">
         <v>148</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
       <c r="G4" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="K4" s="55" t="s">
+      <c r="K4" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="55"/>
+      <c r="L4" s="79"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="70" t="s">
         <v>145</v>
       </c>
-      <c r="B5" s="68"/>
-      <c r="C5" s="71" t="str">
+      <c r="B5" s="71"/>
+      <c r="C5" s="74" t="str">
         <f>IF(OR(ISBLANK(C3),ISBLANK(C4)),"",_xlfn.CONCAT("SW",VLOOKUP(C3,reference!G3:H5,2,FALSE),C4))</f>
         <v/>
       </c>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
       <c r="G5" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="K5" s="73" t="s">
+      <c r="K5" s="76" t="s">
         <v>198</v>
       </c>
-      <c r="L5" s="73"/>
+      <c r="L5" s="76"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="70" t="s">
         <v>138</v>
       </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="79" t="str">
+      <c r="B6" s="71"/>
+      <c r="C6" s="57" t="str">
         <f>IF(OR(ISBLANK(C2),ISBLANK(C3),LEN(C5)=0),"",_xlfn.CONCAT(C2,"_sWGA_",C5))</f>
         <v/>
       </c>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
       <c r="G6" s="34"/>
-      <c r="K6" s="73"/>
-      <c r="L6" s="73"/>
+      <c r="K6" s="76"/>
+      <c r="L6" s="76"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A7" s="83" t="s">
+      <c r="A7" s="61" t="s">
         <v>199</v>
       </c>
-      <c r="B7" s="83"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
       <c r="G7" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A8" s="83" t="s">
+      <c r="A8" s="61" t="s">
         <v>200</v>
       </c>
-      <c r="B8" s="83"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="78"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56"/>
       <c r="G8" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A9" s="84" t="s">
+      <c r="A9" s="62" t="s">
         <v>196</v>
       </c>
-      <c r="B9" s="84"/>
-      <c r="C9" s="82" t="str">
+      <c r="B9" s="62"/>
+      <c r="C9" s="60" t="str">
         <f>IF(OR(LEN(C7)=0, LEN(C8)=0),"",_xlfn.CONCAT(C7,"_Batch",C8))</f>
         <v/>
       </c>
-      <c r="D9" s="82"/>
-      <c r="E9" s="82"/>
-      <c r="F9" s="82"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
       <c r="G9" s="23" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A10" s="84" t="s">
+      <c r="A10" s="62" t="s">
         <v>204</v>
       </c>
-      <c r="B10" s="84"/>
-      <c r="C10" s="85" t="str">
+      <c r="B10" s="62"/>
+      <c r="C10" s="63" t="str">
         <f>IF(OR(LEN(C6)=0,LEN(exp_summary)=0),"",_xlfn.CONCAT(C6,"_",exp_summary,".xlsx"))</f>
         <v/>
       </c>
-      <c r="D10" s="85"/>
-      <c r="E10" s="85"/>
-      <c r="F10" s="85"/>
-      <c r="G10" s="85"/>
-      <c r="H10" s="85"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="65" t="s">
+      <c r="A11" s="54" t="s">
         <v>139</v>
       </c>
-      <c r="B11" s="66"/>
-      <c r="C11" s="78"/>
-      <c r="D11" s="78"/>
-      <c r="E11" s="78"/>
-      <c r="F11" s="78"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
       <c r="G11" s="23" t="s">
         <v>157</v>
       </c>
@@ -2451,10 +2451,10 @@
       <c r="B12" s="44" t="s">
         <v>158</v>
       </c>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="76"/>
+      <c r="C12" s="66"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
       <c r="G12" t="s">
         <v>147</v>
       </c>
@@ -2464,28 +2464,28 @@
       <c r="B13" s="44" t="s">
         <v>194</v>
       </c>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="61"/>
-      <c r="I13" s="61"/>
-      <c r="J13" s="61"/>
-      <c r="K13" s="61"/>
+      <c r="C13" s="85"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="85"/>
+      <c r="F13" s="85"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="85"/>
+      <c r="I13" s="85"/>
+      <c r="J13" s="85"/>
+      <c r="K13" s="85"/>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="42"/>
       <c r="B14" s="44"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="61"/>
-      <c r="H14" s="61"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="61"/>
-      <c r="K14" s="61"/>
+      <c r="C14" s="85"/>
+      <c r="D14" s="85"/>
+      <c r="E14" s="85"/>
+      <c r="F14" s="85"/>
+      <c r="G14" s="85"/>
+      <c r="H14" s="85"/>
+      <c r="I14" s="85"/>
+      <c r="J14" s="85"/>
+      <c r="K14" s="85"/>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="8"/>
@@ -2524,162 +2524,162 @@
       <c r="G17" s="8"/>
     </row>
     <row r="18" spans="1:13" ht="16.5" thickBot="1">
-      <c r="A18" s="80" t="s">
+      <c r="A18" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="80"/>
-      <c r="C18" s="80"/>
-      <c r="D18" s="81" t="s">
+      <c r="B18" s="58"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="81"/>
-      <c r="F18" s="81" t="str">
+      <c r="E18" s="59"/>
+      <c r="F18" s="59" t="str">
         <f>_xlfn.CONCAT("MM x",exp_rxns," (µl)")</f>
         <v>MM x (µl)</v>
       </c>
-      <c r="G18" s="81"/>
-      <c r="J18" s="59" t="s">
+      <c r="G18" s="59"/>
+      <c r="J18" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="K18" s="59"/>
+      <c r="K18" s="83"/>
       <c r="L18" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:13">
-      <c r="A19" s="74" t="s">
+      <c r="A19" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="74"/>
-      <c r="C19" s="74"/>
-      <c r="D19" s="62">
+      <c r="B19" s="65"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="64">
         <v>5</v>
       </c>
-      <c r="E19" s="62"/>
-      <c r="F19" s="77" t="str">
+      <c r="E19" s="64"/>
+      <c r="F19" s="67" t="str">
         <f t="shared" ref="F19:F24" si="0">IF(ISBLANK(swga_rxnvol),"",SUM(D19*exp_rxns*(1+$D$16)))</f>
         <v/>
       </c>
-      <c r="G19" s="77"/>
-      <c r="J19" s="60">
+      <c r="G19" s="67"/>
+      <c r="J19" s="84">
         <v>35</v>
       </c>
-      <c r="K19" s="60"/>
+      <c r="K19" s="84"/>
       <c r="L19" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" s="75" t="s">
+      <c r="A20" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="75"/>
-      <c r="C20" s="75"/>
-      <c r="D20" s="62">
+      <c r="B20" s="53"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="64">
         <v>0.25</v>
       </c>
-      <c r="E20" s="62"/>
-      <c r="F20" s="77" t="str">
+      <c r="E20" s="64"/>
+      <c r="F20" s="67" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G20" s="77"/>
-      <c r="J20" s="60">
+      <c r="G20" s="67"/>
+      <c r="J20" s="84">
         <v>34</v>
       </c>
-      <c r="K20" s="60"/>
+      <c r="K20" s="84"/>
       <c r="L20" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:13">
-      <c r="A21" s="75" t="s">
+      <c r="A21" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="75"/>
-      <c r="C21" s="75"/>
-      <c r="D21" s="62">
+      <c r="B21" s="53"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="64">
         <v>0.125</v>
       </c>
-      <c r="E21" s="62"/>
-      <c r="F21" s="77" t="str">
+      <c r="E21" s="64"/>
+      <c r="F21" s="67" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G21" s="77"/>
-      <c r="J21" s="57">
+      <c r="G21" s="67"/>
+      <c r="J21" s="81">
         <v>33</v>
       </c>
-      <c r="K21" s="57"/>
+      <c r="K21" s="81"/>
       <c r="L21" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:13">
-      <c r="A22" s="74" t="s">
+      <c r="A22" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="74"/>
-      <c r="C22" s="74"/>
-      <c r="D22" s="62">
+      <c r="B22" s="65"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="64">
         <v>5</v>
       </c>
-      <c r="E22" s="62"/>
-      <c r="F22" s="77" t="str">
+      <c r="E22" s="64"/>
+      <c r="F22" s="67" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G22" s="77"/>
-      <c r="J22" s="58">
+      <c r="G22" s="67"/>
+      <c r="J22" s="82">
         <v>32</v>
       </c>
-      <c r="K22" s="58"/>
+      <c r="K22" s="82"/>
       <c r="L22" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:13">
-      <c r="A23" s="75" t="s">
+      <c r="A23" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="75"/>
-      <c r="C23" s="75"/>
-      <c r="D23" s="62">
+      <c r="B23" s="53"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="64">
         <v>8.625</v>
       </c>
-      <c r="E23" s="62"/>
-      <c r="F23" s="77" t="str">
+      <c r="E23" s="64"/>
+      <c r="F23" s="67" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G23" s="77"/>
-      <c r="J23" s="57">
+      <c r="G23" s="67"/>
+      <c r="J23" s="81">
         <v>31</v>
       </c>
-      <c r="K23" s="57"/>
+      <c r="K23" s="81"/>
       <c r="L23" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:13">
-      <c r="A24" s="74" t="s">
+      <c r="A24" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="74"/>
-      <c r="C24" s="74"/>
-      <c r="D24" s="62">
+      <c r="B24" s="65"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="64">
         <v>1</v>
       </c>
-      <c r="E24" s="62"/>
-      <c r="F24" s="77" t="str">
+      <c r="E24" s="64"/>
+      <c r="F24" s="67" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G24" s="77"/>
-      <c r="J24" s="57">
+      <c r="G24" s="67"/>
+      <c r="J24" s="81">
         <v>30</v>
       </c>
-      <c r="K24" s="57"/>
+      <c r="K24" s="81"/>
       <c r="L24" s="7" t="s">
         <v>15</v>
       </c>
@@ -2689,10 +2689,10 @@
         <f>_xlfn.CONCAT("Add ",SUM(D19:D24)," µl of MM to each well")</f>
         <v>Add 20 µl of MM to each well</v>
       </c>
-      <c r="J25" s="57">
+      <c r="J25" s="81">
         <v>65</v>
       </c>
-      <c r="K25" s="57"/>
+      <c r="K25" s="81"/>
       <c r="L25" s="7" t="s">
         <v>18</v>
       </c>
@@ -2702,10 +2702,10 @@
       <c r="C26" s="10"/>
       <c r="D26" s="8"/>
       <c r="G26" s="11"/>
-      <c r="J26" s="57">
+      <c r="J26" s="81">
         <v>10</v>
       </c>
-      <c r="K26" s="57"/>
+      <c r="K26" s="81"/>
       <c r="L26" s="14" t="s">
         <v>13</v>
       </c>
@@ -2720,11 +2720,11 @@
       <c r="D27" s="8"/>
       <c r="F27" s="14"/>
       <c r="G27" s="11"/>
-      <c r="K27" s="53" t="s">
+      <c r="K27" s="77" t="s">
         <v>149</v>
       </c>
-      <c r="L27" s="53"/>
-      <c r="M27" s="53"/>
+      <c r="L27" s="77"/>
+      <c r="M27" s="77"/>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="15" t="s">
@@ -2745,11 +2745,11 @@
       <c r="D29" s="8"/>
       <c r="F29" s="14"/>
       <c r="G29" s="11"/>
-      <c r="K29" s="53" t="s">
+      <c r="K29" s="77" t="s">
         <v>149</v>
       </c>
-      <c r="L29" s="53"/>
-      <c r="M29" s="53"/>
+      <c r="L29" s="77"/>
+      <c r="M29" s="77"/>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="15"/>
@@ -2814,424 +2814,424 @@
       <c r="A33" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="48">
-        <f>sWGA!D3</f>
-        <v>0</v>
-      </c>
-      <c r="C33" s="48">
-        <f>sWGA!D11</f>
-        <v>0</v>
-      </c>
-      <c r="D33" s="48">
-        <f>sWGA!D19</f>
-        <v>0</v>
-      </c>
-      <c r="E33" s="48">
-        <f>sWGA!D27</f>
-        <v>0</v>
-      </c>
-      <c r="F33" s="48">
-        <f>sWGA!D35</f>
-        <v>0</v>
-      </c>
-      <c r="G33" s="48">
-        <f>sWGA!D43</f>
-        <v>0</v>
-      </c>
-      <c r="H33" s="48">
-        <f>sWGA!D51</f>
-        <v>0</v>
-      </c>
-      <c r="I33" s="48">
-        <f>sWGA!D59</f>
-        <v>0</v>
-      </c>
-      <c r="J33" s="48">
-        <f>sWGA!D67</f>
-        <v>0</v>
-      </c>
-      <c r="K33" s="48">
-        <f>sWGA!D75</f>
-        <v>0</v>
-      </c>
-      <c r="L33" s="48">
-        <f>sWGA!D83</f>
-        <v>0</v>
-      </c>
-      <c r="M33" s="48">
-        <f>sWGA!D91</f>
-        <v>0</v>
+      <c r="B33" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D3),"",sWGA!$D3)</f>
+        <v/>
+      </c>
+      <c r="C33" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D11),"",sWGA!$D11)</f>
+        <v/>
+      </c>
+      <c r="D33" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D19),"",sWGA!$D19)</f>
+        <v/>
+      </c>
+      <c r="E33" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D27),"",sWGA!$D27)</f>
+        <v/>
+      </c>
+      <c r="F33" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D35),"",sWGA!$D35)</f>
+        <v/>
+      </c>
+      <c r="G33" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D43),"",sWGA!$D43)</f>
+        <v/>
+      </c>
+      <c r="H33" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D51),"",sWGA!$D51)</f>
+        <v/>
+      </c>
+      <c r="I33" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D59),"",sWGA!$D59)</f>
+        <v/>
+      </c>
+      <c r="J33" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D67),"",sWGA!$D67)</f>
+        <v/>
+      </c>
+      <c r="K33" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D75),"",sWGA!$D75)</f>
+        <v/>
+      </c>
+      <c r="L33" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D83),"",sWGA!$D83)</f>
+        <v/>
+      </c>
+      <c r="M33" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D91),"",sWGA!$D91)</f>
+        <v/>
       </c>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="48">
-        <f>sWGA!D4</f>
-        <v>0</v>
-      </c>
-      <c r="C34" s="48">
-        <f>sWGA!D12</f>
-        <v>0</v>
-      </c>
-      <c r="D34" s="48">
-        <f>sWGA!D20</f>
-        <v>0</v>
-      </c>
-      <c r="E34" s="48">
-        <f>sWGA!D28</f>
-        <v>0</v>
-      </c>
-      <c r="F34" s="48">
-        <f>sWGA!D36</f>
-        <v>0</v>
-      </c>
-      <c r="G34" s="48">
-        <f>sWGA!D44</f>
-        <v>0</v>
-      </c>
-      <c r="H34" s="48">
-        <f>sWGA!D52</f>
-        <v>0</v>
-      </c>
-      <c r="I34" s="48">
-        <f>sWGA!D60</f>
-        <v>0</v>
-      </c>
-      <c r="J34" s="48">
-        <f>sWGA!D68</f>
-        <v>0</v>
-      </c>
-      <c r="K34" s="48">
-        <f>sWGA!D76</f>
-        <v>0</v>
-      </c>
-      <c r="L34" s="48">
-        <f>sWGA!D84</f>
-        <v>0</v>
-      </c>
-      <c r="M34" s="48">
-        <f>sWGA!D92</f>
-        <v>0</v>
+      <c r="B34" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D4),"",sWGA!$D4)</f>
+        <v/>
+      </c>
+      <c r="C34" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D12),"",sWGA!$D12)</f>
+        <v/>
+      </c>
+      <c r="D34" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D20),"",sWGA!$D20)</f>
+        <v/>
+      </c>
+      <c r="E34" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D28),"",sWGA!$D28)</f>
+        <v/>
+      </c>
+      <c r="F34" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D36),"",sWGA!$D36)</f>
+        <v/>
+      </c>
+      <c r="G34" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D44),"",sWGA!$D44)</f>
+        <v/>
+      </c>
+      <c r="H34" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D52),"",sWGA!$D52)</f>
+        <v/>
+      </c>
+      <c r="I34" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D60),"",sWGA!$D60)</f>
+        <v/>
+      </c>
+      <c r="J34" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D68),"",sWGA!$D68)</f>
+        <v/>
+      </c>
+      <c r="K34" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D76),"",sWGA!$D76)</f>
+        <v/>
+      </c>
+      <c r="L34" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D84),"",sWGA!$D84)</f>
+        <v/>
+      </c>
+      <c r="M34" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D92),"",sWGA!$D92)</f>
+        <v/>
       </c>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="48">
-        <f>sWGA!D5</f>
-        <v>0</v>
-      </c>
-      <c r="C35" s="48">
-        <f>sWGA!D13</f>
-        <v>0</v>
-      </c>
-      <c r="D35" s="48">
-        <f>sWGA!D21</f>
-        <v>0</v>
-      </c>
-      <c r="E35" s="48">
-        <f>sWGA!D29</f>
-        <v>0</v>
-      </c>
-      <c r="F35" s="48">
-        <f>sWGA!D37</f>
-        <v>0</v>
-      </c>
-      <c r="G35" s="48">
-        <f>sWGA!D45</f>
-        <v>0</v>
-      </c>
-      <c r="H35" s="48">
-        <f>sWGA!D53</f>
-        <v>0</v>
-      </c>
-      <c r="I35" s="48">
-        <f>sWGA!D61</f>
-        <v>0</v>
-      </c>
-      <c r="J35" s="48">
-        <f>sWGA!D69</f>
-        <v>0</v>
-      </c>
-      <c r="K35" s="48">
-        <f>sWGA!D77</f>
-        <v>0</v>
-      </c>
-      <c r="L35" s="48">
-        <f>sWGA!D85</f>
-        <v>0</v>
-      </c>
-      <c r="M35" s="48">
-        <f>sWGA!D93</f>
-        <v>0</v>
+      <c r="B35" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D5),"",sWGA!$D5)</f>
+        <v/>
+      </c>
+      <c r="C35" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D13),"",sWGA!$D13)</f>
+        <v/>
+      </c>
+      <c r="D35" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D21),"",sWGA!$D21)</f>
+        <v/>
+      </c>
+      <c r="E35" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D29),"",sWGA!$D29)</f>
+        <v/>
+      </c>
+      <c r="F35" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D37),"",sWGA!$D37)</f>
+        <v/>
+      </c>
+      <c r="G35" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D45),"",sWGA!$D45)</f>
+        <v/>
+      </c>
+      <c r="H35" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D53),"",sWGA!$D53)</f>
+        <v/>
+      </c>
+      <c r="I35" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D61),"",sWGA!$D61)</f>
+        <v/>
+      </c>
+      <c r="J35" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D69),"",sWGA!$D69)</f>
+        <v/>
+      </c>
+      <c r="K35" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D77),"",sWGA!$D77)</f>
+        <v/>
+      </c>
+      <c r="L35" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D85),"",sWGA!$D85)</f>
+        <v/>
+      </c>
+      <c r="M35" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D93),"",sWGA!$D93)</f>
+        <v/>
       </c>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="48">
-        <f>sWGA!D6</f>
-        <v>0</v>
-      </c>
-      <c r="C36" s="48">
-        <f>sWGA!D14</f>
-        <v>0</v>
-      </c>
-      <c r="D36" s="48">
-        <f>sWGA!D22</f>
-        <v>0</v>
-      </c>
-      <c r="E36" s="48">
-        <f>sWGA!D30</f>
-        <v>0</v>
-      </c>
-      <c r="F36" s="48">
-        <f>sWGA!D38</f>
-        <v>0</v>
-      </c>
-      <c r="G36" s="48">
-        <f>sWGA!D46</f>
-        <v>0</v>
-      </c>
-      <c r="H36" s="48">
-        <f>sWGA!D54</f>
-        <v>0</v>
-      </c>
-      <c r="I36" s="48">
-        <f>sWGA!D62</f>
-        <v>0</v>
-      </c>
-      <c r="J36" s="48">
-        <f>sWGA!D70</f>
-        <v>0</v>
-      </c>
-      <c r="K36" s="48">
-        <f>sWGA!D78</f>
-        <v>0</v>
-      </c>
-      <c r="L36" s="48">
-        <f>sWGA!D86</f>
-        <v>0</v>
-      </c>
-      <c r="M36" s="48">
-        <f>sWGA!D94</f>
-        <v>0</v>
+      <c r="B36" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D6),"",sWGA!$D6)</f>
+        <v/>
+      </c>
+      <c r="C36" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D14),"",sWGA!$D14)</f>
+        <v/>
+      </c>
+      <c r="D36" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D22),"",sWGA!$D22)</f>
+        <v/>
+      </c>
+      <c r="E36" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D30),"",sWGA!$D30)</f>
+        <v/>
+      </c>
+      <c r="F36" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D38),"",sWGA!$D38)</f>
+        <v/>
+      </c>
+      <c r="G36" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D46),"",sWGA!$D46)</f>
+        <v/>
+      </c>
+      <c r="H36" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D54),"",sWGA!$D54)</f>
+        <v/>
+      </c>
+      <c r="I36" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D62),"",sWGA!$D62)</f>
+        <v/>
+      </c>
+      <c r="J36" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D70),"",sWGA!$D70)</f>
+        <v/>
+      </c>
+      <c r="K36" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D78),"",sWGA!$D78)</f>
+        <v/>
+      </c>
+      <c r="L36" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D86),"",sWGA!$D86)</f>
+        <v/>
+      </c>
+      <c r="M36" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D94),"",sWGA!$D94)</f>
+        <v/>
       </c>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="B37" s="48">
-        <f>sWGA!D7</f>
-        <v>0</v>
-      </c>
-      <c r="C37" s="48">
-        <f>sWGA!D15</f>
-        <v>0</v>
-      </c>
-      <c r="D37" s="48">
-        <f>sWGA!D23</f>
-        <v>0</v>
-      </c>
-      <c r="E37" s="48">
-        <f>sWGA!D31</f>
-        <v>0</v>
-      </c>
-      <c r="F37" s="48">
-        <f>sWGA!D39</f>
-        <v>0</v>
-      </c>
-      <c r="G37" s="48">
-        <f>sWGA!D47</f>
-        <v>0</v>
-      </c>
-      <c r="H37" s="48">
-        <f>sWGA!D55</f>
-        <v>0</v>
-      </c>
-      <c r="I37" s="48">
-        <f>sWGA!D63</f>
-        <v>0</v>
-      </c>
-      <c r="J37" s="48">
-        <f>sWGA!D71</f>
-        <v>0</v>
-      </c>
-      <c r="K37" s="48">
-        <f>sWGA!D79</f>
-        <v>0</v>
-      </c>
-      <c r="L37" s="48">
-        <f>sWGA!D87</f>
-        <v>0</v>
-      </c>
-      <c r="M37" s="48">
-        <f>sWGA!D95</f>
-        <v>0</v>
+      <c r="B37" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D7),"",sWGA!$D7)</f>
+        <v/>
+      </c>
+      <c r="C37" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D15),"",sWGA!$D15)</f>
+        <v/>
+      </c>
+      <c r="D37" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D23),"",sWGA!$D23)</f>
+        <v/>
+      </c>
+      <c r="E37" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D31),"",sWGA!$D31)</f>
+        <v/>
+      </c>
+      <c r="F37" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D39),"",sWGA!$D39)</f>
+        <v/>
+      </c>
+      <c r="G37" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D47),"",sWGA!$D47)</f>
+        <v/>
+      </c>
+      <c r="H37" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D55),"",sWGA!$D55)</f>
+        <v/>
+      </c>
+      <c r="I37" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D63),"",sWGA!$D63)</f>
+        <v/>
+      </c>
+      <c r="J37" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D71),"",sWGA!$D71)</f>
+        <v/>
+      </c>
+      <c r="K37" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D79),"",sWGA!$D79)</f>
+        <v/>
+      </c>
+      <c r="L37" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D87),"",sWGA!$D87)</f>
+        <v/>
+      </c>
+      <c r="M37" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D95),"",sWGA!$D95)</f>
+        <v/>
       </c>
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="48">
-        <f>sWGA!D8</f>
-        <v>0</v>
-      </c>
-      <c r="C38" s="48">
-        <f>sWGA!D16</f>
-        <v>0</v>
-      </c>
-      <c r="D38" s="48">
-        <f>sWGA!D24</f>
-        <v>0</v>
-      </c>
-      <c r="E38" s="48">
-        <f>sWGA!D32</f>
-        <v>0</v>
-      </c>
-      <c r="F38" s="48">
-        <f>sWGA!D40</f>
-        <v>0</v>
-      </c>
-      <c r="G38" s="48">
-        <f>sWGA!D48</f>
-        <v>0</v>
-      </c>
-      <c r="H38" s="48">
-        <f>sWGA!D56</f>
-        <v>0</v>
-      </c>
-      <c r="I38" s="48">
-        <f>sWGA!D64</f>
-        <v>0</v>
-      </c>
-      <c r="J38" s="48">
-        <f>sWGA!D72</f>
-        <v>0</v>
-      </c>
-      <c r="K38" s="48">
-        <f>sWGA!D80</f>
-        <v>0</v>
-      </c>
-      <c r="L38" s="48">
-        <f>sWGA!D88</f>
-        <v>0</v>
-      </c>
-      <c r="M38" s="48">
-        <f>sWGA!D96</f>
-        <v>0</v>
+      <c r="B38" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D8),"",sWGA!$D8)</f>
+        <v/>
+      </c>
+      <c r="C38" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D16),"",sWGA!$D16)</f>
+        <v/>
+      </c>
+      <c r="D38" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D24),"",sWGA!$D24)</f>
+        <v/>
+      </c>
+      <c r="E38" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D32),"",sWGA!$D32)</f>
+        <v/>
+      </c>
+      <c r="F38" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D40),"",sWGA!$D40)</f>
+        <v/>
+      </c>
+      <c r="G38" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D48),"",sWGA!$D48)</f>
+        <v/>
+      </c>
+      <c r="H38" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D56),"",sWGA!$D56)</f>
+        <v/>
+      </c>
+      <c r="I38" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D64),"",sWGA!$D64)</f>
+        <v/>
+      </c>
+      <c r="J38" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D72),"",sWGA!$D72)</f>
+        <v/>
+      </c>
+      <c r="K38" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D80),"",sWGA!$D80)</f>
+        <v/>
+      </c>
+      <c r="L38" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D88),"",sWGA!$D88)</f>
+        <v/>
+      </c>
+      <c r="M38" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D96),"",sWGA!$D96)</f>
+        <v/>
       </c>
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="48">
-        <f>sWGA!D9</f>
-        <v>0</v>
-      </c>
-      <c r="C39" s="48">
-        <f>sWGA!D17</f>
-        <v>0</v>
-      </c>
-      <c r="D39" s="48">
-        <f>sWGA!D25</f>
-        <v>0</v>
-      </c>
-      <c r="E39" s="48">
-        <f>sWGA!D33</f>
-        <v>0</v>
-      </c>
-      <c r="F39" s="48">
-        <f>sWGA!D41</f>
-        <v>0</v>
-      </c>
-      <c r="G39" s="48">
-        <f>sWGA!D49</f>
-        <v>0</v>
-      </c>
-      <c r="H39" s="48">
-        <f>sWGA!D57</f>
-        <v>0</v>
-      </c>
-      <c r="I39" s="48">
-        <f>sWGA!D65</f>
-        <v>0</v>
-      </c>
-      <c r="J39" s="48">
-        <f>sWGA!D73</f>
-        <v>0</v>
-      </c>
-      <c r="K39" s="48">
-        <f>sWGA!D81</f>
-        <v>0</v>
-      </c>
-      <c r="L39" s="48">
-        <f>sWGA!D89</f>
-        <v>0</v>
-      </c>
-      <c r="M39" s="48">
-        <f>sWGA!D97</f>
-        <v>0</v>
+      <c r="B39" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D9),"",sWGA!$D9)</f>
+        <v/>
+      </c>
+      <c r="C39" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D17),"",sWGA!$D17)</f>
+        <v/>
+      </c>
+      <c r="D39" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D25),"",sWGA!$D25)</f>
+        <v/>
+      </c>
+      <c r="E39" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D33),"",sWGA!$D33)</f>
+        <v/>
+      </c>
+      <c r="F39" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D41),"",sWGA!$D41)</f>
+        <v/>
+      </c>
+      <c r="G39" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D49),"",sWGA!$D49)</f>
+        <v/>
+      </c>
+      <c r="H39" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D57),"",sWGA!$D57)</f>
+        <v/>
+      </c>
+      <c r="I39" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D65),"",sWGA!$D65)</f>
+        <v/>
+      </c>
+      <c r="J39" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D73),"",sWGA!$D73)</f>
+        <v/>
+      </c>
+      <c r="K39" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D81),"",sWGA!$D81)</f>
+        <v/>
+      </c>
+      <c r="L39" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D89),"",sWGA!$D89)</f>
+        <v/>
+      </c>
+      <c r="M39" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D97),"",sWGA!$D97)</f>
+        <v/>
       </c>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="B40" s="48">
-        <f>sWGA!D10</f>
-        <v>0</v>
-      </c>
-      <c r="C40" s="48">
-        <f>sWGA!D18</f>
-        <v>0</v>
-      </c>
-      <c r="D40" s="48">
-        <f>sWGA!D26</f>
-        <v>0</v>
-      </c>
-      <c r="E40" s="48">
-        <f>sWGA!D34</f>
-        <v>0</v>
-      </c>
-      <c r="F40" s="48">
-        <f>sWGA!D42</f>
-        <v>0</v>
-      </c>
-      <c r="G40" s="48">
-        <f>sWGA!D50</f>
-        <v>0</v>
-      </c>
-      <c r="H40" s="48">
-        <f>sWGA!D58</f>
-        <v>0</v>
-      </c>
-      <c r="I40" s="48">
-        <f>sWGA!D66</f>
-        <v>0</v>
-      </c>
-      <c r="J40" s="48">
-        <f>sWGA!D74</f>
-        <v>0</v>
-      </c>
-      <c r="K40" s="48">
-        <f>sWGA!D82</f>
-        <v>0</v>
-      </c>
-      <c r="L40" s="48">
-        <f>sWGA!D90</f>
-        <v>0</v>
-      </c>
-      <c r="M40" s="48">
-        <f>sWGA!D98</f>
-        <v>0</v>
+      <c r="B40" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D10),"",sWGA!$D10)</f>
+        <v/>
+      </c>
+      <c r="C40" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D18),"",sWGA!$D18)</f>
+        <v/>
+      </c>
+      <c r="D40" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D26),"",sWGA!$D26)</f>
+        <v/>
+      </c>
+      <c r="E40" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D34),"",sWGA!$D34)</f>
+        <v/>
+      </c>
+      <c r="F40" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D42),"",sWGA!$D42)</f>
+        <v/>
+      </c>
+      <c r="G40" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D50),"",sWGA!$D50)</f>
+        <v/>
+      </c>
+      <c r="H40" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D58),"",sWGA!$D58)</f>
+        <v/>
+      </c>
+      <c r="I40" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D66),"",sWGA!$D66)</f>
+        <v/>
+      </c>
+      <c r="J40" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D74),"",sWGA!$D74)</f>
+        <v/>
+      </c>
+      <c r="K40" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D82),"",sWGA!$D82)</f>
+        <v/>
+      </c>
+      <c r="L40" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D90),"",sWGA!$D90)</f>
+        <v/>
+      </c>
+      <c r="M40" s="48" t="str">
+        <f>IF(ISBLANK(sWGA!$D98),"",sWGA!$D98)</f>
+        <v/>
       </c>
     </row>
     <row r="41" spans="1:13">
@@ -3239,6 +3239,50 @@
     </row>
   </sheetData>
   <mergeCells count="60">
+    <mergeCell ref="K27:M27"/>
+    <mergeCell ref="K29:M29"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="C13:K14"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="K5:L6"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="A11:B11"/>
@@ -3255,50 +3299,6 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C10:H10"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="K5:L6"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="K27:M27"/>
-    <mergeCell ref="K29:M29"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="C13:K14"/>
-    <mergeCell ref="D23:E23"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="C2:C4 C11:C13">
@@ -3355,7 +3355,7 @@
   <dimension ref="A1:J111"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3430,9 +3430,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F3" s="3">
-        <v>10</v>
-      </c>
+      <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="16" t="str">
@@ -3454,9 +3452,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F4" s="3">
-        <v>10</v>
-      </c>
+      <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="16" t="str">
@@ -3478,9 +3474,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F5" s="3">
-        <v>10</v>
-      </c>
+      <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="16" t="str">
@@ -3502,9 +3496,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F6" s="3">
-        <v>10</v>
-      </c>
+      <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="16" t="str">
@@ -3526,9 +3518,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F7" s="3">
-        <v>10</v>
-      </c>
+      <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="16" t="str">
@@ -3550,9 +3540,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F8" s="3">
-        <v>10</v>
-      </c>
+      <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="16" t="str">
@@ -3574,9 +3562,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F9" s="3">
-        <v>10</v>
-      </c>
+      <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="16" t="str">
@@ -3598,9 +3584,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F10" s="3">
-        <v>10</v>
-      </c>
+      <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="16" t="str">
@@ -3622,9 +3606,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F11" s="3">
-        <v>10</v>
-      </c>
+      <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="16" t="str">
@@ -3646,9 +3628,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F12" s="3">
-        <v>10</v>
-      </c>
+      <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="16" t="str">
@@ -3670,9 +3650,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F13" s="3">
-        <v>10</v>
-      </c>
+      <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="16" t="str">
@@ -3694,9 +3672,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F14" s="3">
-        <v>10</v>
-      </c>
+      <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="16" t="str">
@@ -3718,9 +3694,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F15" s="3">
-        <v>10</v>
-      </c>
+      <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="16" t="str">
@@ -3742,9 +3716,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F16" s="3">
-        <v>10</v>
-      </c>
+      <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="16" t="str">
@@ -3766,9 +3738,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F17" s="3">
-        <v>10</v>
-      </c>
+      <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="16" t="str">
@@ -3790,9 +3760,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F18" s="3">
-        <v>10</v>
-      </c>
+      <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="16" t="str">
@@ -3814,9 +3782,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F19" s="3">
-        <v>10</v>
-      </c>
+      <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="16" t="str">
@@ -3838,9 +3804,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F20" s="3">
-        <v>10</v>
-      </c>
+      <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="16" t="str">
@@ -3862,9 +3826,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F21" s="3">
-        <v>10</v>
-      </c>
+      <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="16" t="str">
@@ -3886,9 +3848,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F22" s="3">
-        <v>10</v>
-      </c>
+      <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="16" t="str">
@@ -3910,9 +3870,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F23" s="3">
-        <v>10</v>
-      </c>
+      <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="16" t="str">
@@ -3934,9 +3892,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F24" s="3">
-        <v>10</v>
-      </c>
+      <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="16" t="str">
@@ -3958,9 +3914,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F25" s="3">
-        <v>10</v>
-      </c>
+      <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="16" t="str">
@@ -3982,9 +3936,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F26" s="3">
-        <v>10</v>
-      </c>
+      <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="16" t="str">
@@ -4006,9 +3958,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F27" s="3">
-        <v>10</v>
-      </c>
+      <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="16" t="str">
@@ -4030,9 +3980,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F28" s="3">
-        <v>10</v>
-      </c>
+      <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="16" t="str">
@@ -4054,9 +4002,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F29" s="3">
-        <v>10</v>
-      </c>
+      <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="16" t="str">
@@ -4078,9 +4024,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F30" s="3">
-        <v>10</v>
-      </c>
+      <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="16" t="str">
@@ -4102,9 +4046,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F31" s="3">
-        <v>10</v>
-      </c>
+      <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="16" t="str">
@@ -4126,9 +4068,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F32" s="3">
-        <v>10</v>
-      </c>
+      <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="16" t="str">
@@ -4150,9 +4090,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F33" s="3">
-        <v>10</v>
-      </c>
+      <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="16" t="str">
@@ -4174,9 +4112,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F34" s="3">
-        <v>10</v>
-      </c>
+      <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="16" t="str">
@@ -4198,9 +4134,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F35" s="3">
-        <v>10</v>
-      </c>
+      <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="16" t="str">
@@ -4222,9 +4156,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F36" s="3">
-        <v>10</v>
-      </c>
+      <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="16" t="str">
@@ -4246,9 +4178,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F37" s="3">
-        <v>10</v>
-      </c>
+      <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="16" t="str">
@@ -4270,9 +4200,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F38" s="3">
-        <v>10</v>
-      </c>
+      <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="16" t="str">
@@ -4294,9 +4222,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F39" s="3">
-        <v>10</v>
-      </c>
+      <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="16" t="str">
@@ -4318,9 +4244,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F40" s="3">
-        <v>10</v>
-      </c>
+      <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="16" t="str">
@@ -4342,9 +4266,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F41" s="3">
-        <v>10</v>
-      </c>
+      <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="16" t="str">
@@ -4366,9 +4288,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F42" s="3">
-        <v>10</v>
-      </c>
+      <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="16" t="str">
@@ -4390,9 +4310,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F43" s="3">
-        <v>10</v>
-      </c>
+      <c r="F43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="16" t="str">
@@ -4414,9 +4332,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F44" s="3">
-        <v>10</v>
-      </c>
+      <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="16" t="str">
@@ -4438,9 +4354,7 @@
         <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
-      <c r="F45" s="3">
-        <v>10</v>
-      </c>
+      <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="16" t="str">
@@ -5807,7 +5721,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -6228,9 +6142,9 @@
         <f>IF(LEN(sWGA!E3)=0,"",sWGA!E3)</f>
         <v/>
       </c>
-      <c r="E2">
+      <c r="E2" t="str">
         <f>IF(LEN(sWGA!F3)=0,"",sWGA!F3)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F2" t="str">
         <f>IF(LEN(sWGA!I3)=0,"",sWGA!I3)</f>
@@ -6254,9 +6168,9 @@
         <f>IF(LEN(sWGA!E4)=0,"",sWGA!E4)</f>
         <v/>
       </c>
-      <c r="E3">
+      <c r="E3" t="str">
         <f>IF(LEN(sWGA!F4)=0,"",sWGA!F4)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F3" t="str">
         <f>IF(LEN(sWGA!I4)=0,"",sWGA!I4)</f>
@@ -6280,9 +6194,9 @@
         <f>IF(LEN(sWGA!E5)=0,"",sWGA!E5)</f>
         <v/>
       </c>
-      <c r="E4">
+      <c r="E4" t="str">
         <f>IF(LEN(sWGA!F5)=0,"",sWGA!F5)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F4" t="str">
         <f>IF(LEN(sWGA!I5)=0,"",sWGA!I5)</f>
@@ -6306,9 +6220,9 @@
         <f>IF(LEN(sWGA!E6)=0,"",sWGA!E6)</f>
         <v/>
       </c>
-      <c r="E5">
+      <c r="E5" t="str">
         <f>IF(LEN(sWGA!F6)=0,"",sWGA!F6)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F5" t="str">
         <f>IF(LEN(sWGA!I6)=0,"",sWGA!I6)</f>
@@ -6332,9 +6246,9 @@
         <f>IF(LEN(sWGA!E7)=0,"",sWGA!E7)</f>
         <v/>
       </c>
-      <c r="E6">
+      <c r="E6" t="str">
         <f>IF(LEN(sWGA!F7)=0,"",sWGA!F7)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F6" t="str">
         <f>IF(LEN(sWGA!I7)=0,"",sWGA!I7)</f>
@@ -6358,9 +6272,9 @@
         <f>IF(LEN(sWGA!E8)=0,"",sWGA!E8)</f>
         <v/>
       </c>
-      <c r="E7">
+      <c r="E7" t="str">
         <f>IF(LEN(sWGA!F8)=0,"",sWGA!F8)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F7" t="str">
         <f>IF(LEN(sWGA!I8)=0,"",sWGA!I8)</f>
@@ -6384,9 +6298,9 @@
         <f>IF(LEN(sWGA!E9)=0,"",sWGA!E9)</f>
         <v/>
       </c>
-      <c r="E8">
+      <c r="E8" t="str">
         <f>IF(LEN(sWGA!F9)=0,"",sWGA!F9)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F8" t="str">
         <f>IF(LEN(sWGA!I9)=0,"",sWGA!I9)</f>
@@ -6410,9 +6324,9 @@
         <f>IF(LEN(sWGA!E10)=0,"",sWGA!E10)</f>
         <v/>
       </c>
-      <c r="E9">
+      <c r="E9" t="str">
         <f>IF(LEN(sWGA!F10)=0,"",sWGA!F10)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F9" t="str">
         <f>IF(LEN(sWGA!I10)=0,"",sWGA!I10)</f>
@@ -6436,9 +6350,9 @@
         <f>IF(LEN(sWGA!E11)=0,"",sWGA!E11)</f>
         <v/>
       </c>
-      <c r="E10">
+      <c r="E10" t="str">
         <f>IF(LEN(sWGA!F11)=0,"",sWGA!F11)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F10" t="str">
         <f>IF(LEN(sWGA!I11)=0,"",sWGA!I11)</f>
@@ -6462,9 +6376,9 @@
         <f>IF(LEN(sWGA!E12)=0,"",sWGA!E12)</f>
         <v/>
       </c>
-      <c r="E11">
+      <c r="E11" t="str">
         <f>IF(LEN(sWGA!F12)=0,"",sWGA!F12)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F11" t="str">
         <f>IF(LEN(sWGA!I12)=0,"",sWGA!I12)</f>
@@ -6488,9 +6402,9 @@
         <f>IF(LEN(sWGA!E13)=0,"",sWGA!E13)</f>
         <v/>
       </c>
-      <c r="E12">
+      <c r="E12" t="str">
         <f>IF(LEN(sWGA!F13)=0,"",sWGA!F13)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F12" t="str">
         <f>IF(LEN(sWGA!I13)=0,"",sWGA!I13)</f>
@@ -6514,9 +6428,9 @@
         <f>IF(LEN(sWGA!E14)=0,"",sWGA!E14)</f>
         <v/>
       </c>
-      <c r="E13">
+      <c r="E13" t="str">
         <f>IF(LEN(sWGA!F14)=0,"",sWGA!F14)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F13" t="str">
         <f>IF(LEN(sWGA!I14)=0,"",sWGA!I14)</f>
@@ -6540,9 +6454,9 @@
         <f>IF(LEN(sWGA!E15)=0,"",sWGA!E15)</f>
         <v/>
       </c>
-      <c r="E14">
+      <c r="E14" t="str">
         <f>IF(LEN(sWGA!F15)=0,"",sWGA!F15)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F14" t="str">
         <f>IF(LEN(sWGA!I15)=0,"",sWGA!I15)</f>
@@ -6566,9 +6480,9 @@
         <f>IF(LEN(sWGA!E16)=0,"",sWGA!E16)</f>
         <v/>
       </c>
-      <c r="E15">
+      <c r="E15" t="str">
         <f>IF(LEN(sWGA!F16)=0,"",sWGA!F16)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F15" t="str">
         <f>IF(LEN(sWGA!I16)=0,"",sWGA!I16)</f>
@@ -6592,9 +6506,9 @@
         <f>IF(LEN(sWGA!E17)=0,"",sWGA!E17)</f>
         <v/>
       </c>
-      <c r="E16">
+      <c r="E16" t="str">
         <f>IF(LEN(sWGA!F17)=0,"",sWGA!F17)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F16" t="str">
         <f>IF(LEN(sWGA!I17)=0,"",sWGA!I17)</f>
@@ -6618,9 +6532,9 @@
         <f>IF(LEN(sWGA!E18)=0,"",sWGA!E18)</f>
         <v/>
       </c>
-      <c r="E17">
+      <c r="E17" t="str">
         <f>IF(LEN(sWGA!F18)=0,"",sWGA!F18)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F17" t="str">
         <f>IF(LEN(sWGA!I18)=0,"",sWGA!I18)</f>
@@ -6644,9 +6558,9 @@
         <f>IF(LEN(sWGA!E19)=0,"",sWGA!E19)</f>
         <v/>
       </c>
-      <c r="E18">
+      <c r="E18" t="str">
         <f>IF(LEN(sWGA!F19)=0,"",sWGA!F19)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F18" t="str">
         <f>IF(LEN(sWGA!I19)=0,"",sWGA!I19)</f>
@@ -6670,9 +6584,9 @@
         <f>IF(LEN(sWGA!E20)=0,"",sWGA!E20)</f>
         <v/>
       </c>
-      <c r="E19">
+      <c r="E19" t="str">
         <f>IF(LEN(sWGA!F20)=0,"",sWGA!F20)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F19" t="str">
         <f>IF(LEN(sWGA!I20)=0,"",sWGA!I20)</f>
@@ -6696,9 +6610,9 @@
         <f>IF(LEN(sWGA!E21)=0,"",sWGA!E21)</f>
         <v/>
       </c>
-      <c r="E20">
+      <c r="E20" t="str">
         <f>IF(LEN(sWGA!F21)=0,"",sWGA!F21)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F20" t="str">
         <f>IF(LEN(sWGA!I21)=0,"",sWGA!I21)</f>
@@ -6722,9 +6636,9 @@
         <f>IF(LEN(sWGA!E22)=0,"",sWGA!E22)</f>
         <v/>
       </c>
-      <c r="E21">
+      <c r="E21" t="str">
         <f>IF(LEN(sWGA!F22)=0,"",sWGA!F22)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F21" t="str">
         <f>IF(LEN(sWGA!I22)=0,"",sWGA!I22)</f>
@@ -6748,9 +6662,9 @@
         <f>IF(LEN(sWGA!E23)=0,"",sWGA!E23)</f>
         <v/>
       </c>
-      <c r="E22">
+      <c r="E22" t="str">
         <f>IF(LEN(sWGA!F23)=0,"",sWGA!F23)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F22" t="str">
         <f>IF(LEN(sWGA!I23)=0,"",sWGA!I23)</f>
@@ -6774,9 +6688,9 @@
         <f>IF(LEN(sWGA!E24)=0,"",sWGA!E24)</f>
         <v/>
       </c>
-      <c r="E23">
+      <c r="E23" t="str">
         <f>IF(LEN(sWGA!F24)=0,"",sWGA!F24)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F23" t="str">
         <f>IF(LEN(sWGA!I24)=0,"",sWGA!I24)</f>
@@ -6800,9 +6714,9 @@
         <f>IF(LEN(sWGA!E25)=0,"",sWGA!E25)</f>
         <v/>
       </c>
-      <c r="E24">
+      <c r="E24" t="str">
         <f>IF(LEN(sWGA!F25)=0,"",sWGA!F25)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F24" t="str">
         <f>IF(LEN(sWGA!I25)=0,"",sWGA!I25)</f>
@@ -6826,9 +6740,9 @@
         <f>IF(LEN(sWGA!E26)=0,"",sWGA!E26)</f>
         <v/>
       </c>
-      <c r="E25">
+      <c r="E25" t="str">
         <f>IF(LEN(sWGA!F26)=0,"",sWGA!F26)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F25" t="str">
         <f>IF(LEN(sWGA!I26)=0,"",sWGA!I26)</f>
@@ -6852,9 +6766,9 @@
         <f>IF(LEN(sWGA!E27)=0,"",sWGA!E27)</f>
         <v/>
       </c>
-      <c r="E26">
+      <c r="E26" t="str">
         <f>IF(LEN(sWGA!F27)=0,"",sWGA!F27)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F26" t="str">
         <f>IF(LEN(sWGA!I27)=0,"",sWGA!I27)</f>
@@ -6878,9 +6792,9 @@
         <f>IF(LEN(sWGA!E28)=0,"",sWGA!E28)</f>
         <v/>
       </c>
-      <c r="E27">
+      <c r="E27" t="str">
         <f>IF(LEN(sWGA!F28)=0,"",sWGA!F28)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F27" t="str">
         <f>IF(LEN(sWGA!I28)=0,"",sWGA!I28)</f>
@@ -6904,9 +6818,9 @@
         <f>IF(LEN(sWGA!E29)=0,"",sWGA!E29)</f>
         <v/>
       </c>
-      <c r="E28">
+      <c r="E28" t="str">
         <f>IF(LEN(sWGA!F29)=0,"",sWGA!F29)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F28" t="str">
         <f>IF(LEN(sWGA!I29)=0,"",sWGA!I29)</f>
@@ -6930,9 +6844,9 @@
         <f>IF(LEN(sWGA!E30)=0,"",sWGA!E30)</f>
         <v/>
       </c>
-      <c r="E29">
+      <c r="E29" t="str">
         <f>IF(LEN(sWGA!F30)=0,"",sWGA!F30)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F29" t="str">
         <f>IF(LEN(sWGA!I30)=0,"",sWGA!I30)</f>
@@ -6956,9 +6870,9 @@
         <f>IF(LEN(sWGA!E31)=0,"",sWGA!E31)</f>
         <v/>
       </c>
-      <c r="E30">
+      <c r="E30" t="str">
         <f>IF(LEN(sWGA!F31)=0,"",sWGA!F31)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F30" t="str">
         <f>IF(LEN(sWGA!I31)=0,"",sWGA!I31)</f>
@@ -6982,9 +6896,9 @@
         <f>IF(LEN(sWGA!E32)=0,"",sWGA!E32)</f>
         <v/>
       </c>
-      <c r="E31">
+      <c r="E31" t="str">
         <f>IF(LEN(sWGA!F32)=0,"",sWGA!F32)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F31" t="str">
         <f>IF(LEN(sWGA!I32)=0,"",sWGA!I32)</f>
@@ -7008,9 +6922,9 @@
         <f>IF(LEN(sWGA!E33)=0,"",sWGA!E33)</f>
         <v/>
       </c>
-      <c r="E32">
+      <c r="E32" t="str">
         <f>IF(LEN(sWGA!F33)=0,"",sWGA!F33)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F32" t="str">
         <f>IF(LEN(sWGA!I33)=0,"",sWGA!I33)</f>
@@ -7034,9 +6948,9 @@
         <f>IF(LEN(sWGA!E34)=0,"",sWGA!E34)</f>
         <v/>
       </c>
-      <c r="E33">
+      <c r="E33" t="str">
         <f>IF(LEN(sWGA!F34)=0,"",sWGA!F34)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F33" t="str">
         <f>IF(LEN(sWGA!I34)=0,"",sWGA!I34)</f>
@@ -7060,9 +6974,9 @@
         <f>IF(LEN(sWGA!E35)=0,"",sWGA!E35)</f>
         <v/>
       </c>
-      <c r="E34">
+      <c r="E34" t="str">
         <f>IF(LEN(sWGA!F35)=0,"",sWGA!F35)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F34" t="str">
         <f>IF(LEN(sWGA!I35)=0,"",sWGA!I35)</f>
@@ -7086,9 +7000,9 @@
         <f>IF(LEN(sWGA!E36)=0,"",sWGA!E36)</f>
         <v/>
       </c>
-      <c r="E35">
+      <c r="E35" t="str">
         <f>IF(LEN(sWGA!F36)=0,"",sWGA!F36)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F35" t="str">
         <f>IF(LEN(sWGA!I36)=0,"",sWGA!I36)</f>
@@ -7112,9 +7026,9 @@
         <f>IF(LEN(sWGA!E37)=0,"",sWGA!E37)</f>
         <v/>
       </c>
-      <c r="E36">
+      <c r="E36" t="str">
         <f>IF(LEN(sWGA!F37)=0,"",sWGA!F37)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F36" t="str">
         <f>IF(LEN(sWGA!I37)=0,"",sWGA!I37)</f>
@@ -7138,9 +7052,9 @@
         <f>IF(LEN(sWGA!E38)=0,"",sWGA!E38)</f>
         <v/>
       </c>
-      <c r="E37">
+      <c r="E37" t="str">
         <f>IF(LEN(sWGA!F38)=0,"",sWGA!F38)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F37" t="str">
         <f>IF(LEN(sWGA!I38)=0,"",sWGA!I38)</f>
@@ -7164,9 +7078,9 @@
         <f>IF(LEN(sWGA!E39)=0,"",sWGA!E39)</f>
         <v/>
       </c>
-      <c r="E38">
+      <c r="E38" t="str">
         <f>IF(LEN(sWGA!F39)=0,"",sWGA!F39)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F38" t="str">
         <f>IF(LEN(sWGA!I39)=0,"",sWGA!I39)</f>
@@ -7190,9 +7104,9 @@
         <f>IF(LEN(sWGA!E40)=0,"",sWGA!E40)</f>
         <v/>
       </c>
-      <c r="E39">
+      <c r="E39" t="str">
         <f>IF(LEN(sWGA!F40)=0,"",sWGA!F40)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F39" t="str">
         <f>IF(LEN(sWGA!I40)=0,"",sWGA!I40)</f>
@@ -7216,9 +7130,9 @@
         <f>IF(LEN(sWGA!E41)=0,"",sWGA!E41)</f>
         <v/>
       </c>
-      <c r="E40">
+      <c r="E40" t="str">
         <f>IF(LEN(sWGA!F41)=0,"",sWGA!F41)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F40" t="str">
         <f>IF(LEN(sWGA!I41)=0,"",sWGA!I41)</f>
@@ -7242,9 +7156,9 @@
         <f>IF(LEN(sWGA!E42)=0,"",sWGA!E42)</f>
         <v/>
       </c>
-      <c r="E41">
+      <c r="E41" t="str">
         <f>IF(LEN(sWGA!F42)=0,"",sWGA!F42)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F41" t="str">
         <f>IF(LEN(sWGA!I42)=0,"",sWGA!I42)</f>
@@ -7268,9 +7182,9 @@
         <f>IF(LEN(sWGA!E43)=0,"",sWGA!E43)</f>
         <v/>
       </c>
-      <c r="E42">
+      <c r="E42" t="str">
         <f>IF(LEN(sWGA!F43)=0,"",sWGA!F43)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F42" t="str">
         <f>IF(LEN(sWGA!I43)=0,"",sWGA!I43)</f>
@@ -7294,9 +7208,9 @@
         <f>IF(LEN(sWGA!E44)=0,"",sWGA!E44)</f>
         <v/>
       </c>
-      <c r="E43">
+      <c r="E43" t="str">
         <f>IF(LEN(sWGA!F44)=0,"",sWGA!F44)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F43" t="str">
         <f>IF(LEN(sWGA!I44)=0,"",sWGA!I44)</f>
@@ -7320,9 +7234,9 @@
         <f>IF(LEN(sWGA!E45)=0,"",sWGA!E45)</f>
         <v/>
       </c>
-      <c r="E44">
+      <c r="E44" t="str">
         <f>IF(LEN(sWGA!F45)=0,"",sWGA!F45)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F44" t="str">
         <f>IF(LEN(sWGA!I45)=0,"",sWGA!I45)</f>

</xml_diff>

<commit_message>
Updated templates and example data better structured
</commit_message>
<xml_diff>
--- a/resources/templates/NOMADS_sWGA_Worksheet.xlsx
+++ b/resources/templates/NOMADS_sWGA_Worksheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitrepos\warehouse\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A314AB-CB6E-470F-B3CB-5EE549B29FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D739CBC-B493-4A51-A690-D9265D6D4DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{202E2ACC-7D07-5944-B6D6-A1D8A2363375}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="34080" windowHeight="22200" xr2:uid="{202E2ACC-7D07-5944-B6D6-A1D8A2363375}"/>
   </bookViews>
   <sheets>
     <sheet name="Assay" sheetId="6" r:id="rId1"/>
@@ -36,8 +36,9 @@
     <definedName name="swga_notes">Assay!$C$13</definedName>
     <definedName name="swga_rxnvol">Assay!$C$12</definedName>
     <definedName name="swga_targetmass">reference!$B$3</definedName>
+    <definedName name="swga_template_maxvol">reference!$B$4</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -79,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="225">
   <si>
     <t>ng</t>
   </si>
@@ -88,9 +89,6 @@
   </si>
   <si>
     <t>SWGA</t>
-  </si>
-  <si>
-    <t>10x Phi29</t>
   </si>
   <si>
     <t>10mM dNTP</t>
@@ -239,30 +237,6 @@
   </si>
   <si>
     <t>#</t>
-  </si>
-  <si>
-    <r>
-      <t>1000</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>µ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>M Primer Mix</t>
-    </r>
   </si>
   <si>
     <t>A1</t>
@@ -674,32 +648,6 @@
     <t xml:space="preserve">  3. Run sWGA on thermocycler according to above right table</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">  3.Quantify 1 µl (199 µl WS 1X HS DNA). Dilute in H</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>O if required</t>
-    </r>
-  </si>
-  <si>
     <t>sWGA template (ul)</t>
   </si>
   <si>
@@ -935,6 +883,50 @@
   <si>
     <t>1. Select a complete entry i.e. for names you would highlight two cells e.g. G5 and H5</t>
   </si>
+  <si>
+    <t>Changelog from previous version</t>
+  </si>
+  <si>
+    <t>Changed all CONCAT refs to CONCATENATE for translations</t>
+  </si>
+  <si>
+    <t>10x Phi29 Buffer</t>
+  </si>
+  <si>
+    <t>100nM Primer Mix</t>
+  </si>
+  <si>
+    <t>swga template max vol</t>
+  </si>
+  <si>
+    <t>ul</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  4. Quantify 1 µl (199 µl WS 1X HS DNA). Dilute in H</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>O if required</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -944,9 +936,16 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1279,14 +1278,14 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1297,31 +1296,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1331,23 +1330,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1360,13 +1359,13 @@
     <xf numFmtId="165" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1378,7 +1377,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1386,8 +1385,8 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1398,22 +1397,22 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1421,58 +1420,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="1" fontId="8" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="8" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1481,57 +1489,49 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma" xfId="5" builtinId="3"/>
@@ -1690,7 +1690,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1876,7 +1876,7 @@
     <tableColumn id="2" xr3:uid="{CE61E1E1-E9B3-4D58-9DFE-1AB6DDFCD05A}" name="Sample ID" dataDxfId="12"/>
     <tableColumn id="3" xr3:uid="{9795EF0E-2DE1-455A-A3FF-0804F7CBA8C3}" name="Extraction ID" dataDxfId="11"/>
     <tableColumn id="7" xr3:uid="{AE7E794D-3E11-4B03-8051-B54164DF087E}" name="sWGA Identifier" dataDxfId="10">
-      <calculatedColumnFormula>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{17E17A49-9A1B-4B36-98B0-66368F2A095E}" name="sWGA template (ul)" dataDxfId="9"/>
     <tableColumn id="12" xr3:uid="{6392E74F-2A5C-4E61-A4E5-54FD59E2FF90}" name="sWGA qubit [DNA] (ng / ul)" dataDxfId="8"/>
@@ -1957,9 +1957,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1997,7 +1997,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2103,7 +2103,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2245,7 +2245,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2259,8 +2259,8 @@
   </sheetPr>
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2269,220 +2269,220 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="63" t="s">
-        <v>150</v>
-      </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
+      <c r="A1" s="68" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="54" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="55"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="69" t="s">
+        <v>139</v>
+      </c>
+      <c r="H2" s="69"/>
+      <c r="K2" s="80" t="s">
+        <v>138</v>
+      </c>
+      <c r="L2" s="80"/>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A3" s="54" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3" s="55"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" t="s">
+        <v>145</v>
+      </c>
+      <c r="K3" s="78" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="78"/>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A4" s="54" t="s">
+        <v>146</v>
+      </c>
+      <c r="B4" s="55"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="K4" s="79" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="79"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="70" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="71"/>
+      <c r="C5" s="74" t="str">
+        <f>IF(OR(ISBLANK(C3),ISBLANK(C4)),"",CONCATENATE("SW",VLOOKUP(C3,reference!G3:H5,2,FALSE),C4))</f>
+        <v/>
+      </c>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="K5" s="76" t="s">
+        <v>194</v>
+      </c>
+      <c r="L5" s="76"/>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A6" s="70" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" s="71"/>
+      <c r="C6" s="57" t="str">
+        <f>IF(OR(ISBLANK(C2),ISBLANK(C3),LEN(C5)=0),"",CONCATENATE(C2,"_sWGA_",C5))</f>
+        <v/>
+      </c>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="34"/>
+      <c r="K6" s="76"/>
+      <c r="L6" s="76"/>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A7" s="61" t="s">
+        <v>195</v>
+      </c>
+      <c r="B7" s="61"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A8" s="61" t="s">
+        <v>196</v>
+      </c>
+      <c r="B8" s="61"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56"/>
+      <c r="G8" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A9" s="62" t="s">
+        <v>192</v>
+      </c>
+      <c r="B9" s="62"/>
+      <c r="C9" s="60" t="str">
+        <f>IF(OR(LEN(C7)=0, LEN(C8)=0),"",CONCATENATE(C7,"_Batch",C8))</f>
+        <v/>
+      </c>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="23" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A10" s="62" t="s">
+        <v>200</v>
+      </c>
+      <c r="B10" s="62"/>
+      <c r="C10" s="63" t="str">
+        <f>IF(OR(LEN(C6)=0,LEN(exp_summary)=0),"",CONCATENATE(C6,"_",exp_summary,".xlsx"))</f>
+        <v/>
+      </c>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="54" t="s">
         <v>137</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="64" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="64"/>
-      <c r="K2" s="56" t="s">
-        <v>140</v>
-      </c>
-      <c r="L2" s="56"/>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A3" s="65" t="s">
-        <v>142</v>
-      </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" t="s">
-        <v>147</v>
-      </c>
-      <c r="K3" s="54" t="s">
-        <v>6</v>
-      </c>
-      <c r="L3" s="54"/>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A4" s="65" t="s">
-        <v>148</v>
-      </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="37" t="s">
-        <v>146</v>
-      </c>
-      <c r="K4" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="L4" s="55"/>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="67" t="s">
-        <v>145</v>
-      </c>
-      <c r="B5" s="68"/>
-      <c r="C5" s="71" t="str">
-        <f>IF(OR(ISBLANK(C3),ISBLANK(C4)),"",_xlfn.CONCAT("SW",VLOOKUP(C3,reference!G3:H5,2,FALSE),C4))</f>
-        <v/>
-      </c>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="K5" s="73" t="s">
-        <v>197</v>
-      </c>
-      <c r="L5" s="73"/>
-    </row>
-    <row r="6" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A6" s="67" t="s">
-        <v>138</v>
-      </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="79" t="str">
-        <f>IF(OR(ISBLANK(C2),ISBLANK(C3),LEN(C5)=0),"",_xlfn.CONCAT(C2,"_sWGA_",C5))</f>
-        <v/>
-      </c>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
-      <c r="G6" s="34"/>
-      <c r="K6" s="73"/>
-      <c r="L6" s="73"/>
-    </row>
-    <row r="7" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A7" s="83" t="s">
-        <v>198</v>
-      </c>
-      <c r="B7" s="83"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
-      <c r="G7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A8" s="83" t="s">
-        <v>199</v>
-      </c>
-      <c r="B8" s="83"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="78"/>
-      <c r="G8" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A9" s="84" t="s">
-        <v>195</v>
-      </c>
-      <c r="B9" s="84"/>
-      <c r="C9" s="82" t="str">
-        <f>IF(OR(LEN(C7)=0, LEN(C8)=0),"",_xlfn.CONCAT(C7,"_Batch",C8))</f>
-        <v/>
-      </c>
-      <c r="D9" s="82"/>
-      <c r="E9" s="82"/>
-      <c r="F9" s="82"/>
-      <c r="G9" s="23" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A10" s="84" t="s">
-        <v>203</v>
-      </c>
-      <c r="B10" s="84"/>
-      <c r="C10" s="85" t="str">
-        <f>IF(OR(LEN(C6)=0,LEN(exp_summary)=0),"",_xlfn.CONCAT(C6,"_",exp_summary,".xlsx"))</f>
-        <v/>
-      </c>
-      <c r="D10" s="85"/>
-      <c r="E10" s="85"/>
-      <c r="F10" s="85"/>
-      <c r="G10" s="85"/>
-      <c r="H10" s="85"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="65" t="s">
-        <v>139</v>
-      </c>
-      <c r="B11" s="66"/>
-      <c r="C11" s="78"/>
-      <c r="D11" s="78"/>
-      <c r="E11" s="78"/>
-      <c r="F11" s="78"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
       <c r="G11" s="23" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="42"/>
       <c r="B12" s="44" t="s">
-        <v>158</v>
-      </c>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="76"/>
+        <v>156</v>
+      </c>
+      <c r="C12" s="66"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
       <c r="G12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="42"/>
       <c r="B13" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="61"/>
-      <c r="I13" s="61"/>
-      <c r="J13" s="61"/>
-      <c r="K13" s="61"/>
+        <v>190</v>
+      </c>
+      <c r="C13" s="85"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="85"/>
+      <c r="F13" s="85"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="85"/>
+      <c r="I13" s="85"/>
+      <c r="J13" s="85"/>
+      <c r="K13" s="85"/>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="42"/>
       <c r="B14" s="44"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="61"/>
-      <c r="H14" s="61"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="61"/>
-      <c r="K14" s="61"/>
+      <c r="C14" s="85"/>
+      <c r="D14" s="85"/>
+      <c r="E14" s="85"/>
+      <c r="F14" s="85"/>
+      <c r="G14" s="85"/>
+      <c r="H14" s="85"/>
+      <c r="I14" s="85"/>
+      <c r="J14" s="85"/>
+      <c r="K14" s="85"/>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="8"/>
@@ -2495,11 +2495,11 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" s="18">
         <v>0.1</v>
@@ -2510,8 +2510,8 @@
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="15" t="str">
-        <f>_xlfn.CONCAT("  1. Make up master mix as below and add ", SUM(D19:D24), " µl to each well")</f>
-        <v xml:space="preserve">  1. Make up master mix as below and add 20 µl to each well</v>
+        <f>CONCATENATE("  1. Make up master mix as below and add ", SUM(D19:D24), " µl to each well")</f>
+        <v xml:space="preserve">  1. Make up master mix as below and add -10 µl to each well</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="8"/>
@@ -2521,177 +2521,179 @@
       <c r="G17" s="8"/>
     </row>
     <row r="18" spans="1:13" ht="16.5" thickBot="1">
-      <c r="A18" s="80" t="s">
+      <c r="A18" s="58" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="58"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="80"/>
-      <c r="C18" s="80"/>
-      <c r="D18" s="81" t="s">
+      <c r="E18" s="59"/>
+      <c r="F18" s="59" t="str">
+        <f>CONCATENATE("MM x",exp_rxns," (µl)")</f>
+        <v>MM x (µl)</v>
+      </c>
+      <c r="G18" s="59"/>
+      <c r="J18" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="81"/>
-      <c r="F18" s="81" t="str">
-        <f>_xlfn.CONCAT("MM x",exp_rxns," (µl)")</f>
-        <v>MM x (µl)</v>
-      </c>
-      <c r="G18" s="81"/>
-      <c r="J18" s="59" t="s">
+      <c r="K18" s="83"/>
+      <c r="L18" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="K18" s="59"/>
-      <c r="L18" s="13" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="19" spans="1:13">
-      <c r="A19" s="74" t="s">
+      <c r="A19" s="65" t="s">
+        <v>220</v>
+      </c>
+      <c r="B19" s="65"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="64">
+        <f>swga_rxnvol/10</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="64"/>
+      <c r="F19" s="67" t="str">
+        <f t="shared" ref="F19:F22" si="0">IF(ISBLANK(swga_rxnvol),"",SUM(D19*exp_rxns*(1+$D$16)))</f>
+        <v/>
+      </c>
+      <c r="G19" s="67"/>
+      <c r="J19" s="84">
+        <v>35</v>
+      </c>
+      <c r="K19" s="84"/>
+      <c r="L19" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="53"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="64">
+        <v>0.25</v>
+      </c>
+      <c r="E20" s="64"/>
+      <c r="F20" s="67" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G20" s="67"/>
+      <c r="J20" s="84">
+        <v>34</v>
+      </c>
+      <c r="K20" s="84"/>
+      <c r="L20" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="53" t="s">
+        <v>221</v>
+      </c>
+      <c r="B21" s="53"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="64">
+        <v>1.25</v>
+      </c>
+      <c r="E21" s="64"/>
+      <c r="F21" s="67" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G21" s="67"/>
+      <c r="J21" s="81">
+        <v>33</v>
+      </c>
+      <c r="K21" s="81"/>
+      <c r="L21" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="74"/>
-      <c r="C19" s="74"/>
-      <c r="D19" s="62">
+      <c r="B22" s="65"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="64">
         <v>5</v>
       </c>
-      <c r="E19" s="62"/>
-      <c r="F19" s="77" t="str">
-        <f t="shared" ref="F19:F24" si="0">IF(ISBLANK(swga_rxnvol),"",SUM(D19*exp_rxns*(1+$D$16)))</f>
-        <v/>
-      </c>
-      <c r="G19" s="77"/>
-      <c r="J19" s="60">
-        <v>35</v>
-      </c>
-      <c r="K19" s="60"/>
-      <c r="L19" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" s="75" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="75"/>
-      <c r="C20" s="75"/>
-      <c r="D20" s="62">
-        <v>0.25</v>
-      </c>
-      <c r="E20" s="62"/>
-      <c r="F20" s="77" t="str">
+      <c r="E22" s="64"/>
+      <c r="F22" s="67" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G20" s="77"/>
-      <c r="J20" s="60">
-        <v>34</v>
-      </c>
-      <c r="K20" s="60"/>
-      <c r="L20" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="A21" s="75" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="75"/>
-      <c r="C21" s="75"/>
-      <c r="D21" s="62">
-        <v>0.125</v>
-      </c>
-      <c r="E21" s="62"/>
-      <c r="F21" s="77" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G21" s="77"/>
-      <c r="J21" s="57">
-        <v>33</v>
-      </c>
-      <c r="K21" s="57"/>
-      <c r="L21" s="7" t="s">
+      <c r="G22" s="67"/>
+      <c r="J22" s="82">
+        <v>32</v>
+      </c>
+      <c r="K22" s="82"/>
+      <c r="L22" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
-      <c r="A22" s="74" t="s">
+    <row r="23" spans="1:13">
+      <c r="A23" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="74"/>
-      <c r="C22" s="74"/>
-      <c r="D22" s="62">
-        <v>5</v>
-      </c>
-      <c r="E22" s="62"/>
-      <c r="F22" s="77" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G22" s="77"/>
-      <c r="J22" s="58">
-        <v>32</v>
-      </c>
-      <c r="K22" s="58"/>
-      <c r="L22" s="8" t="s">
+      <c r="B23" s="65"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="64">
+        <v>1</v>
+      </c>
+      <c r="E23" s="64"/>
+      <c r="F23" s="67" t="str">
+        <f>IF(ISBLANK(swga_rxnvol),"",SUM(D23*exp_rxns*(1+$D$16)))</f>
+        <v/>
+      </c>
+      <c r="G23" s="67"/>
+      <c r="J23" s="81">
+        <v>31</v>
+      </c>
+      <c r="K23" s="81"/>
+      <c r="L23" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
-      <c r="A23" s="75" t="s">
+    <row r="24" spans="1:13">
+      <c r="A24" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="53"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="64">
+        <f>SUM(swga_rxnvol-swga_template_maxvol)-SUM(D19:E23)</f>
+        <v>-17.5</v>
+      </c>
+      <c r="E24" s="64"/>
+      <c r="F24" s="67" t="str">
+        <f>IF(ISBLANK(swga_rxnvol),"",SUM(D24*exp_rxns*(1+$D$16)))</f>
+        <v/>
+      </c>
+      <c r="G24" s="67"/>
+      <c r="J24" s="81">
+        <v>30</v>
+      </c>
+      <c r="K24" s="81"/>
+      <c r="L24" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="B23" s="75"/>
-      <c r="C23" s="75"/>
-      <c r="D23" s="62">
-        <v>8.625</v>
-      </c>
-      <c r="E23" s="62"/>
-      <c r="F23" s="77" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G23" s="77"/>
-      <c r="J23" s="57">
-        <v>31</v>
-      </c>
-      <c r="K23" s="57"/>
-      <c r="L23" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13">
-      <c r="A24" s="74" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="74"/>
-      <c r="C24" s="74"/>
-      <c r="D24" s="62">
-        <v>1</v>
-      </c>
-      <c r="E24" s="62"/>
-      <c r="F24" s="77" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G24" s="77"/>
-      <c r="J24" s="57">
-        <v>30</v>
-      </c>
-      <c r="K24" s="57"/>
-      <c r="L24" s="7" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:13">
       <c r="G25" s="20" t="str">
-        <f>_xlfn.CONCAT("Add ",SUM(D19:D24)," µl of MM to each well")</f>
-        <v>Add 20 µl of MM to each well</v>
-      </c>
-      <c r="J25" s="57">
+        <f>CONCATENATE("Add ",SUM(D19:D24)," µl of MM to each well")</f>
+        <v>Add -10 µl of MM to each well</v>
+      </c>
+      <c r="J25" s="81">
         <v>65</v>
       </c>
-      <c r="K25" s="57"/>
+      <c r="K25" s="81"/>
       <c r="L25" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -2699,33 +2701,33 @@
       <c r="C26" s="10"/>
       <c r="D26" s="8"/>
       <c r="G26" s="11"/>
-      <c r="J26" s="57">
+      <c r="J26" s="81">
         <v>10</v>
       </c>
-      <c r="K26" s="57"/>
+      <c r="K26" s="81"/>
       <c r="L26" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="15" t="str">
-        <f>_xlfn.CONCAT("  2. For each sample add target of ",swga_targetmass," ng of DNA for each up to a max vol of ",SUM(swga_rxnvol-SUM(D19:E24)),"ul. Add TE as required.")</f>
-        <v xml:space="preserve">  2. For each sample add target of 40 ng of DNA for each up to a max vol of -20ul. Add TE as required.</v>
+        <f>CONCATENATE("  2. For each sample add target of ",swga_targetmass," ng of DNA for each up to a max vol of ",swga_template_maxvol,"ul. Add TE as required.")</f>
+        <v xml:space="preserve">  2. For each sample add target of 40 ng of DNA for each up to a max vol of 10ul. Add TE as required.</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="10"/>
       <c r="D27" s="8"/>
       <c r="F27" s="14"/>
       <c r="G27" s="11"/>
-      <c r="K27" s="53" t="s">
-        <v>149</v>
-      </c>
-      <c r="L27" s="53"/>
-      <c r="M27" s="53"/>
+      <c r="K27" s="77" t="s">
+        <v>147</v>
+      </c>
+      <c r="L27" s="77"/>
+      <c r="M27" s="77"/>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="10"/>
@@ -2735,18 +2737,18 @@
     </row>
     <row r="29" spans="1:13" ht="18.75">
       <c r="A29" s="15" t="s">
-        <v>162</v>
+        <v>224</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="10"/>
       <c r="D29" s="8"/>
       <c r="F29" s="14"/>
       <c r="G29" s="11"/>
-      <c r="K29" s="53" t="s">
-        <v>149</v>
-      </c>
-      <c r="L29" s="53"/>
-      <c r="M29" s="53"/>
+      <c r="K29" s="77" t="s">
+        <v>147</v>
+      </c>
+      <c r="L29" s="77"/>
+      <c r="M29" s="77"/>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="15"/>
@@ -2758,7 +2760,7 @@
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -2809,7 +2811,7 @@
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B33" s="48" t="str">
         <f>IF(ISBLANK(sWGA!$D3),"",sWGA!$D3)</f>
@@ -2862,7 +2864,7 @@
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="41" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B34" s="48" t="str">
         <f>IF(ISBLANK(sWGA!$D4),"",sWGA!$D4)</f>
@@ -2915,7 +2917,7 @@
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="41" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B35" s="48" t="str">
         <f>IF(ISBLANK(sWGA!$D5),"",sWGA!$D5)</f>
@@ -2968,7 +2970,7 @@
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="41" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B36" s="48" t="str">
         <f>IF(ISBLANK(sWGA!$D6),"",sWGA!$D6)</f>
@@ -3021,7 +3023,7 @@
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="41" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B37" s="48" t="str">
         <f>IF(ISBLANK(sWGA!$D7),"",sWGA!$D7)</f>
@@ -3074,7 +3076,7 @@
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B38" s="48" t="str">
         <f>IF(ISBLANK(sWGA!$D8),"",sWGA!$D8)</f>
@@ -3127,7 +3129,7 @@
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="41" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B39" s="48" t="str">
         <f>IF(ISBLANK(sWGA!$D9),"",sWGA!$D9)</f>
@@ -3180,7 +3182,7 @@
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B40" s="48" t="str">
         <f>IF(ISBLANK(sWGA!$D10),"",sWGA!$D10)</f>
@@ -3236,6 +3238,50 @@
     </row>
   </sheetData>
   <mergeCells count="60">
+    <mergeCell ref="K27:M27"/>
+    <mergeCell ref="K29:M29"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="C13:K14"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="K5:L6"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="A11:B11"/>
@@ -3252,52 +3298,8 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C10:H10"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="K5:L6"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="K27:M27"/>
-    <mergeCell ref="K29:M29"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="C13:K14"/>
-    <mergeCell ref="D23:E23"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="C2:C4 C11:C13">
     <cfRule type="expression" dxfId="3" priority="14">
       <formula>COUNTIF(C2,"")</formula>
@@ -3351,8 +3353,8 @@
   </sheetPr>
   <dimension ref="A1:J111"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3370,7 +3372,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="C1" s="86" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" s="87"/>
       <c r="E1" s="88" t="s">
@@ -3384,34 +3386,34 @@
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="48.75" customHeight="1">
       <c r="A2" s="29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" s="47" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F2" s="31" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G2" s="31" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I2" s="31" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J2" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1">
@@ -3419,12 +3421,12 @@
         <v>1</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C3" s="43"/>
       <c r="D3" s="49"/>
       <c r="E3" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F3" s="3"/>
@@ -3441,12 +3443,12 @@
         <v>2</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" s="43"/>
       <c r="D4" s="49"/>
       <c r="E4" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F4" s="3"/>
@@ -3463,12 +3465,12 @@
         <v>3</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C5" s="43"/>
       <c r="D5" s="49"/>
       <c r="E5" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F5" s="3"/>
@@ -3485,12 +3487,12 @@
         <v>4</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C6" s="43"/>
       <c r="D6" s="49"/>
       <c r="E6" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F6" s="3"/>
@@ -3507,12 +3509,12 @@
         <v>5</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C7" s="43"/>
       <c r="D7" s="49"/>
       <c r="E7" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F7" s="3"/>
@@ -3529,12 +3531,12 @@
         <v>6</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C8" s="43"/>
       <c r="D8" s="49"/>
       <c r="E8" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F8" s="3"/>
@@ -3551,12 +3553,12 @@
         <v>7</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C9" s="43"/>
       <c r="D9" s="49"/>
       <c r="E9" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F9" s="3"/>
@@ -3573,12 +3575,12 @@
         <v>8</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C10" s="43"/>
       <c r="D10" s="49"/>
       <c r="E10" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F10" s="3"/>
@@ -3595,12 +3597,12 @@
         <v>9</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C11" s="43"/>
       <c r="D11" s="49"/>
       <c r="E11" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F11" s="3"/>
@@ -3617,12 +3619,12 @@
         <v>10</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C12" s="43"/>
       <c r="D12" s="49"/>
       <c r="E12" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F12" s="3"/>
@@ -3639,12 +3641,12 @@
         <v>11</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C13" s="43"/>
       <c r="D13" s="49"/>
       <c r="E13" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F13" s="3"/>
@@ -3661,12 +3663,12 @@
         <v>12</v>
       </c>
       <c r="B14" s="33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C14" s="43"/>
       <c r="D14" s="49"/>
       <c r="E14" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F14" s="3"/>
@@ -3683,12 +3685,12 @@
         <v>13</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C15" s="43"/>
       <c r="D15" s="49"/>
       <c r="E15" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F15" s="3"/>
@@ -3705,12 +3707,12 @@
         <v>14</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C16" s="43"/>
       <c r="D16" s="49"/>
       <c r="E16" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F16" s="3"/>
@@ -3727,12 +3729,12 @@
         <v>15</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C17" s="43"/>
       <c r="D17" s="49"/>
       <c r="E17" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F17" s="3"/>
@@ -3749,12 +3751,12 @@
         <v>16</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C18" s="43"/>
       <c r="D18" s="49"/>
       <c r="E18" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F18" s="3"/>
@@ -3771,12 +3773,12 @@
         <v>17</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C19" s="43"/>
       <c r="D19" s="49"/>
       <c r="E19" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F19" s="3"/>
@@ -3793,12 +3795,12 @@
         <v>18</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C20" s="43"/>
       <c r="D20" s="49"/>
       <c r="E20" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F20" s="3"/>
@@ -3815,12 +3817,12 @@
         <v>19</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C21" s="43"/>
       <c r="D21" s="49"/>
       <c r="E21" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F21" s="3"/>
@@ -3837,12 +3839,12 @@
         <v>20</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C22" s="43"/>
       <c r="D22" s="49"/>
       <c r="E22" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F22" s="3"/>
@@ -3859,12 +3861,12 @@
         <v>21</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C23" s="43"/>
       <c r="D23" s="49"/>
       <c r="E23" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F23" s="3"/>
@@ -3881,12 +3883,12 @@
         <v>22</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C24" s="43"/>
       <c r="D24" s="49"/>
       <c r="E24" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F24" s="3"/>
@@ -3903,12 +3905,12 @@
         <v>23</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C25" s="43"/>
       <c r="D25" s="49"/>
       <c r="E25" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F25" s="3"/>
@@ -3925,12 +3927,12 @@
         <v>24</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C26" s="43"/>
       <c r="D26" s="49"/>
       <c r="E26" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F26" s="3"/>
@@ -3947,12 +3949,12 @@
         <v>25</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C27" s="43"/>
       <c r="D27" s="49"/>
       <c r="E27" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F27" s="3"/>
@@ -3969,12 +3971,12 @@
         <v>26</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C28" s="43"/>
       <c r="D28" s="49"/>
       <c r="E28" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F28" s="3"/>
@@ -3991,12 +3993,12 @@
         <v>27</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C29" s="43"/>
       <c r="D29" s="49"/>
       <c r="E29" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F29" s="3"/>
@@ -4013,12 +4015,12 @@
         <v>28</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C30" s="43"/>
       <c r="D30" s="49"/>
       <c r="E30" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F30" s="3"/>
@@ -4035,12 +4037,12 @@
         <v>29</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C31" s="43"/>
       <c r="D31" s="49"/>
       <c r="E31" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F31" s="3"/>
@@ -4057,12 +4059,12 @@
         <v>30</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C32" s="43"/>
       <c r="D32" s="49"/>
       <c r="E32" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F32" s="3"/>
@@ -4079,12 +4081,12 @@
         <v>31</v>
       </c>
       <c r="B33" s="25" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C33" s="43"/>
       <c r="D33" s="49"/>
       <c r="E33" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F33" s="3"/>
@@ -4101,12 +4103,12 @@
         <v>32</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C34" s="43"/>
       <c r="D34" s="49"/>
       <c r="E34" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F34" s="3"/>
@@ -4123,12 +4125,12 @@
         <v>33</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C35" s="43"/>
       <c r="D35" s="49"/>
       <c r="E35" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F35" s="3"/>
@@ -4145,12 +4147,12 @@
         <v>34</v>
       </c>
       <c r="B36" s="25" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C36" s="43"/>
       <c r="D36" s="49"/>
       <c r="E36" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F36" s="3"/>
@@ -4167,12 +4169,12 @@
         <v>35</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C37" s="43"/>
       <c r="D37" s="49"/>
       <c r="E37" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F37" s="3"/>
@@ -4189,12 +4191,12 @@
         <v>36</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C38" s="43"/>
       <c r="D38" s="49"/>
       <c r="E38" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F38" s="3"/>
@@ -4211,12 +4213,12 @@
         <v>37</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C39" s="43"/>
       <c r="D39" s="49"/>
       <c r="E39" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F39" s="3"/>
@@ -4233,12 +4235,12 @@
         <v>38</v>
       </c>
       <c r="B40" s="25" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C40" s="43"/>
       <c r="D40" s="49"/>
       <c r="E40" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F40" s="3"/>
@@ -4255,12 +4257,12 @@
         <v>39</v>
       </c>
       <c r="B41" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C41" s="43"/>
       <c r="D41" s="49"/>
       <c r="E41" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F41" s="3"/>
@@ -4277,12 +4279,12 @@
         <v>40</v>
       </c>
       <c r="B42" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C42" s="43"/>
       <c r="D42" s="49"/>
       <c r="E42" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F42" s="3"/>
@@ -4299,12 +4301,12 @@
         <v>41</v>
       </c>
       <c r="B43" s="25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C43" s="43"/>
       <c r="D43" s="49"/>
       <c r="E43" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F43" s="3"/>
@@ -4321,12 +4323,12 @@
         <v>42</v>
       </c>
       <c r="B44" s="25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C44" s="43"/>
       <c r="D44" s="49"/>
       <c r="E44" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F44" s="3"/>
@@ -4343,12 +4345,12 @@
         <v>43</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C45" s="43"/>
       <c r="D45" s="49"/>
       <c r="E45" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F45" s="3"/>
@@ -4365,12 +4367,12 @@
         <v>44</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C46" s="43"/>
       <c r="D46" s="49"/>
       <c r="E46" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F46" s="3"/>
@@ -4387,12 +4389,12 @@
         <v>45</v>
       </c>
       <c r="B47" s="25" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C47" s="43"/>
       <c r="D47" s="49"/>
       <c r="E47" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F47" s="3"/>
@@ -4409,12 +4411,12 @@
         <v>46</v>
       </c>
       <c r="B48" s="25" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C48" s="43"/>
       <c r="D48" s="49"/>
       <c r="E48" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F48" s="3"/>
@@ -4431,12 +4433,12 @@
         <v>47</v>
       </c>
       <c r="B49" s="25" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C49" s="43"/>
       <c r="D49" s="49"/>
       <c r="E49" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F49" s="3"/>
@@ -4453,12 +4455,12 @@
         <v>48</v>
       </c>
       <c r="B50" s="25" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C50" s="43"/>
       <c r="D50" s="49"/>
       <c r="E50" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F50" s="3"/>
@@ -4475,12 +4477,12 @@
         <v>49</v>
       </c>
       <c r="B51" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C51" s="43"/>
       <c r="D51" s="49"/>
       <c r="E51" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F51" s="3"/>
@@ -4497,12 +4499,12 @@
         <v>50</v>
       </c>
       <c r="B52" s="25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C52" s="43"/>
       <c r="D52" s="49"/>
       <c r="E52" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F52" s="3"/>
@@ -4519,12 +4521,12 @@
         <v>51</v>
       </c>
       <c r="B53" s="25" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C53" s="43"/>
       <c r="D53" s="49"/>
       <c r="E53" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F53" s="3"/>
@@ -4541,12 +4543,12 @@
         <v>52</v>
       </c>
       <c r="B54" s="25" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C54" s="43"/>
       <c r="D54" s="49"/>
       <c r="E54" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F54" s="3"/>
@@ -4563,12 +4565,12 @@
         <v>53</v>
       </c>
       <c r="B55" s="25" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C55" s="43"/>
       <c r="D55" s="49"/>
       <c r="E55" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F55" s="3"/>
@@ -4585,12 +4587,12 @@
         <v>54</v>
       </c>
       <c r="B56" s="25" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C56" s="43"/>
       <c r="D56" s="49"/>
       <c r="E56" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F56" s="3"/>
@@ -4607,12 +4609,12 @@
         <v>55</v>
       </c>
       <c r="B57" s="25" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C57" s="43"/>
       <c r="D57" s="49"/>
       <c r="E57" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F57" s="3"/>
@@ -4629,12 +4631,12 @@
         <v>56</v>
       </c>
       <c r="B58" s="25" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C58" s="43"/>
       <c r="D58" s="49"/>
       <c r="E58" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F58" s="3"/>
@@ -4651,12 +4653,12 @@
         <v>57</v>
       </c>
       <c r="B59" s="25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C59" s="43"/>
       <c r="D59" s="49"/>
       <c r="E59" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F59" s="3"/>
@@ -4673,12 +4675,12 @@
         <v>58</v>
       </c>
       <c r="B60" s="25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C60" s="43"/>
       <c r="D60" s="49"/>
       <c r="E60" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F60" s="3"/>
@@ -4695,12 +4697,12 @@
         <v>59</v>
       </c>
       <c r="B61" s="25" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C61" s="43"/>
       <c r="D61" s="49"/>
       <c r="E61" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F61" s="3"/>
@@ -4717,12 +4719,12 @@
         <v>60</v>
       </c>
       <c r="B62" s="25" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C62" s="43"/>
       <c r="D62" s="49"/>
       <c r="E62" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F62" s="3"/>
@@ -4739,12 +4741,12 @@
         <v>61</v>
       </c>
       <c r="B63" s="25" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C63" s="43"/>
       <c r="D63" s="49"/>
       <c r="E63" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F63" s="3"/>
@@ -4761,12 +4763,12 @@
         <v>62</v>
       </c>
       <c r="B64" s="25" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C64" s="43"/>
       <c r="D64" s="49"/>
       <c r="E64" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F64" s="3"/>
@@ -4783,12 +4785,12 @@
         <v>63</v>
       </c>
       <c r="B65" s="25" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C65" s="43"/>
       <c r="D65" s="49"/>
       <c r="E65" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F65" s="3"/>
@@ -4805,12 +4807,12 @@
         <v>64</v>
       </c>
       <c r="B66" s="25" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C66" s="43"/>
       <c r="D66" s="49"/>
       <c r="E66" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F66" s="3"/>
@@ -4827,12 +4829,12 @@
         <v>65</v>
       </c>
       <c r="B67" s="25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C67" s="43"/>
       <c r="D67" s="49"/>
       <c r="E67" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F67" s="3"/>
@@ -4849,12 +4851,12 @@
         <v>66</v>
       </c>
       <c r="B68" s="25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C68" s="43"/>
       <c r="D68" s="49"/>
       <c r="E68" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F68" s="3"/>
@@ -4871,12 +4873,12 @@
         <v>67</v>
       </c>
       <c r="B69" s="25" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C69" s="43"/>
       <c r="D69" s="49"/>
       <c r="E69" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F69" s="3"/>
@@ -4893,12 +4895,12 @@
         <v>68</v>
       </c>
       <c r="B70" s="25" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C70" s="43"/>
       <c r="D70" s="49"/>
       <c r="E70" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F70" s="3"/>
@@ -4915,12 +4917,12 @@
         <v>69</v>
       </c>
       <c r="B71" s="25" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C71" s="43"/>
       <c r="D71" s="49"/>
       <c r="E71" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F71" s="3"/>
@@ -4937,12 +4939,12 @@
         <v>70</v>
       </c>
       <c r="B72" s="25" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C72" s="43"/>
       <c r="D72" s="49"/>
       <c r="E72" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F72" s="3"/>
@@ -4959,12 +4961,12 @@
         <v>71</v>
       </c>
       <c r="B73" s="25" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C73" s="43"/>
       <c r="D73" s="49"/>
       <c r="E73" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F73" s="3"/>
@@ -4981,12 +4983,12 @@
         <v>72</v>
       </c>
       <c r="B74" s="25" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C74" s="43"/>
       <c r="D74" s="49"/>
       <c r="E74" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F74" s="3"/>
@@ -5003,12 +5005,12 @@
         <v>73</v>
       </c>
       <c r="B75" s="25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C75" s="43"/>
       <c r="D75" s="49"/>
       <c r="E75" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F75" s="3"/>
@@ -5025,12 +5027,12 @@
         <v>74</v>
       </c>
       <c r="B76" s="25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C76" s="43"/>
       <c r="D76" s="49"/>
       <c r="E76" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F76" s="3"/>
@@ -5047,12 +5049,12 @@
         <v>75</v>
       </c>
       <c r="B77" s="25" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C77" s="43"/>
       <c r="D77" s="49"/>
       <c r="E77" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F77" s="3"/>
@@ -5069,12 +5071,12 @@
         <v>76</v>
       </c>
       <c r="B78" s="25" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C78" s="43"/>
       <c r="D78" s="49"/>
       <c r="E78" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F78" s="3"/>
@@ -5091,12 +5093,12 @@
         <v>77</v>
       </c>
       <c r="B79" s="25" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C79" s="43"/>
       <c r="D79" s="49"/>
       <c r="E79" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F79" s="3"/>
@@ -5113,12 +5115,12 @@
         <v>78</v>
       </c>
       <c r="B80" s="25" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C80" s="43"/>
       <c r="D80" s="49"/>
       <c r="E80" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F80" s="3"/>
@@ -5135,12 +5137,12 @@
         <v>79</v>
       </c>
       <c r="B81" s="25" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C81" s="43"/>
       <c r="D81" s="49"/>
       <c r="E81" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F81" s="3"/>
@@ -5157,12 +5159,12 @@
         <v>80</v>
       </c>
       <c r="B82" s="25" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C82" s="43"/>
       <c r="D82" s="49"/>
       <c r="E82" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F82" s="3"/>
@@ -5179,12 +5181,12 @@
         <v>81</v>
       </c>
       <c r="B83" s="25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C83" s="43"/>
       <c r="D83" s="49"/>
       <c r="E83" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F83" s="3"/>
@@ -5201,12 +5203,12 @@
         <v>82</v>
       </c>
       <c r="B84" s="25" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C84" s="43"/>
       <c r="D84" s="49"/>
       <c r="E84" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F84" s="3"/>
@@ -5223,12 +5225,12 @@
         <v>83</v>
       </c>
       <c r="B85" s="25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C85" s="43"/>
       <c r="D85" s="49"/>
       <c r="E85" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F85" s="3"/>
@@ -5245,12 +5247,12 @@
         <v>84</v>
       </c>
       <c r="B86" s="25" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C86" s="43"/>
       <c r="D86" s="49"/>
       <c r="E86" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F86" s="3"/>
@@ -5267,12 +5269,12 @@
         <v>85</v>
       </c>
       <c r="B87" s="25" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C87" s="43"/>
       <c r="D87" s="49"/>
       <c r="E87" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F87" s="3"/>
@@ -5289,12 +5291,12 @@
         <v>86</v>
       </c>
       <c r="B88" s="25" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C88" s="43"/>
       <c r="D88" s="49"/>
       <c r="E88" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F88" s="3"/>
@@ -5311,12 +5313,12 @@
         <v>87</v>
       </c>
       <c r="B89" s="25" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C89" s="43"/>
       <c r="D89" s="49"/>
       <c r="E89" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F89" s="3"/>
@@ -5333,12 +5335,12 @@
         <v>88</v>
       </c>
       <c r="B90" s="25" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C90" s="43"/>
       <c r="D90" s="49"/>
       <c r="E90" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F90" s="3"/>
@@ -5355,12 +5357,12 @@
         <v>89</v>
       </c>
       <c r="B91" s="25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C91" s="43"/>
       <c r="D91" s="49"/>
       <c r="E91" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F91" s="3"/>
@@ -5377,12 +5379,12 @@
         <v>90</v>
       </c>
       <c r="B92" s="25" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C92" s="43"/>
       <c r="D92" s="49"/>
       <c r="E92" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F92" s="3"/>
@@ -5399,12 +5401,12 @@
         <v>91</v>
       </c>
       <c r="B93" s="25" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C93" s="43"/>
       <c r="D93" s="49"/>
       <c r="E93" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F93" s="3"/>
@@ -5421,12 +5423,12 @@
         <v>92</v>
       </c>
       <c r="B94" s="25" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C94" s="43"/>
       <c r="D94" s="49"/>
       <c r="E94" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F94" s="3"/>
@@ -5443,12 +5445,12 @@
         <v>93</v>
       </c>
       <c r="B95" s="25" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C95" s="43"/>
       <c r="D95" s="49"/>
       <c r="E95" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F95" s="3"/>
@@ -5465,12 +5467,12 @@
         <v>94</v>
       </c>
       <c r="B96" s="25" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C96" s="43"/>
       <c r="D96" s="49"/>
       <c r="E96" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F96" s="3"/>
@@ -5487,12 +5489,12 @@
         <v>95</v>
       </c>
       <c r="B97" s="25" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C97" s="43"/>
       <c r="D97" s="49"/>
       <c r="E97" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F97" s="3"/>
@@ -5509,12 +5511,12 @@
         <v>96</v>
       </c>
       <c r="B98" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C98" s="43"/>
       <c r="D98" s="49"/>
       <c r="E98" s="38" t="str">
-        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",_xlfn.CONCAT(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
+        <f>IF(SUM(LEN(tbl_sWGA[[#This Row],[Sample ID]])+LEN(tbl_sWGA[[#This Row],[Extraction ID]]))=0,"",CONCATENATE(exp_id,"_",tbl_sWGA[[#This Row],[Well]]))</f>
         <v/>
       </c>
       <c r="F98" s="27"/>
@@ -5683,7 +5685,7 @@
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:J1"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="C3:C98">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text=" ">
       <formula>NOT(ISERROR(SEARCH(" ",C3)))</formula>
@@ -5717,7 +5719,7 @@
   </sheetPr>
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -5734,77 +5736,77 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="39" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="40" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="45" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="45" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="23" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="46" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="46" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B8" s="40" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="46" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="40" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="40" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="40" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="40" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -5821,7 +5823,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -5843,34 +5845,34 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="16.5" thickBot="1">
       <c r="A2" s="35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="36"/>
       <c r="C2" s="36"/>
       <c r="E2" s="35" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G2" s="50" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H2" s="50" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J2" s="50" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>40</v>
@@ -5882,88 +5884,101 @@
         <v>30</v>
       </c>
       <c r="G3" s="51" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="H3" s="51" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J3" s="51" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="2"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="6"/>
+      <c r="A4" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B4" s="17">
+        <v>10</v>
+      </c>
+      <c r="C4" s="90" t="s">
+        <v>223</v>
+      </c>
       <c r="D4" s="6"/>
       <c r="E4">
         <v>50</v>
       </c>
       <c r="G4" s="51" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H4" s="51" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J4" s="51" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="18.75">
       <c r="E5" s="5"/>
       <c r="G5" s="51" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="H5" s="51" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="J5" s="51" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="16.5" thickBot="1">
       <c r="A6" s="35" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B6" s="36"/>
       <c r="C6" s="36"/>
       <c r="G6" s="52" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" s="52" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G8" s="52" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="G9" s="52" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="16.5" thickBot="1">
+      <c r="A10" s="35" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="10" spans="1:14">
       <c r="G10" s="52" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="31.5" customHeight="1">
+      <c r="A11" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="31.5" customHeight="1"/>
     <row r="12" spans="1:14">
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
@@ -5995,34 +6010,34 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D1" t="s">
         <v>185</v>
       </c>
-      <c r="B1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>186</v>
       </c>
-      <c r="D1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E1" t="s">
-        <v>189</v>
-      </c>
       <c r="F1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="J1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -6044,7 +6059,7 @@
       </c>
       <c r="E2">
         <f>exp_version</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2">
         <f>exp_rxns</f>
@@ -6068,7 +6083,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -6099,22 +6114,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:6">

</xml_diff>